<commit_message>
Cambiando nombres campos entidades
</commit_message>
<xml_diff>
--- a/Diccionario de errores.xlsx
+++ b/Diccionario de errores.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">Diccionario de errores</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">Rol ya existe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha final debe ser mayor a la fecha inicial</t>
   </si>
 </sst>
 </file>
@@ -118,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -139,6 +146,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,7 +212,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -297,15 +305,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:D31"/>
+  <dimension ref="B2:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.92"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,6 +527,17 @@
       </c>
       <c r="D31" s="0" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix diccionario de errores
</commit_message>
<xml_diff>
--- a/Diccionario de errores.xlsx
+++ b/Diccionario de errores.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Diccionario de errores</t>
   </si>
   <si>
-    <t xml:space="preserve">NF</t>
+    <t xml:space="preserve">Not Found (NF-)</t>
   </si>
   <si>
     <t xml:space="preserve">Sin usuarios en la DB</t>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">No existe el rol</t>
   </si>
   <si>
-    <t xml:space="preserve">BL</t>
+    <t xml:space="preserve">Business Logic (BL-)</t>
   </si>
   <si>
     <t xml:space="preserve">Nombre de usuario ya existe</t>
@@ -106,7 +106,7 @@
     <t xml:space="preserve">Rol ya existe</t>
   </si>
   <si>
-    <t xml:space="preserve">BR</t>
+    <t xml:space="preserve">Bad Request (BR-)</t>
   </si>
   <si>
     <t xml:space="preserve">Credenciales inválidas</t>
@@ -122,7 +122,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -146,21 +146,41 @@
     </font>
     <font>
       <b val="true"/>
+      <u val="single"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFDE59"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="14">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -169,9 +189,30 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right/>
-      <top style="thin">
+      <top style="hair">
         <color rgb="FF2A6099"/>
       </top>
       <bottom/>
@@ -179,9 +220,67 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left/>
+      <right style="thin"/>
+      <top style="hair">
+        <color rgb="FF2A6099"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
       <right/>
       <top style="thin"/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -210,7 +309,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,15 +318,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,7 +424,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFDE59"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -308,259 +451,279 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:D33"/>
+  <dimension ref="B1:C33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AMJ1048576" activeCellId="0" sqref="AMJ1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="44.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.26"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="30.86"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1024" min="6" style="0" width="11.56"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="0" t="n">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3" t="n">
         <v>101</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2" t="n">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="5" t="n">
         <v>200</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="3" t="n">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="3" t="n">
         <v>201</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="0" t="n">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3" t="n">
         <v>202</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="0" t="n">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="3" t="n">
         <v>203</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="n">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="3" t="n">
         <v>204</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="n">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="3" t="n">
         <v>205</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="4" t="n">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="7" t="n">
         <v>300</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="3" t="n">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="3" t="n">
         <v>301</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="n">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="3" t="n">
         <v>302</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="C14" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="4" t="n">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="7" t="n">
         <v>400</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="C15" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="n">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="3" t="n">
         <v>401</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="4" t="n">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="7" t="n">
         <v>500</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="C17" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="n">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="3" t="n">
         <v>501</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="C18" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="4" t="n">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="7" t="n">
         <v>600</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="C19" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="n">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="3" t="n">
         <v>601</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="C20" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="4" t="n">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="7" t="n">
         <v>700</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="n">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9" t="n">
         <v>701</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="C22" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="C24" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="9" t="n">
         <v>101</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="C25" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="n">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="C26" s="13" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9" t="n">
+        <v>600</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="n">
-        <v>400</v>
-      </c>
-      <c r="D29" s="0" t="s">
-        <v>25</v>
+      <c r="B29" s="9" t="n">
+        <v>700</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="n">
-        <v>600</v>
-      </c>
-      <c r="D30" s="0" t="s">
-        <v>26</v>
-      </c>
+      <c r="B30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="0" t="n">
-        <v>700</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>27</v>
+      <c r="B31" s="14" t="n">
+        <v>100</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="0" t="n">
+      <c r="B32" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="C32" s="13" t="s">
         <v>30</v>
       </c>
     </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:D2"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B30:C30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPágina &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding GET ALL endpoint - Features
</commit_message>
<xml_diff>
--- a/Diccionario de errores.xlsx
+++ b/Diccionario de errores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t xml:space="preserve">Diccionario de errores</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">No existe el rol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin caracteristicas registradas en la DB</t>
   </si>
   <si>
     <t xml:space="preserve">Business Logic (BL-)</t>
@@ -451,19 +454,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:C33"/>
+  <dimension ref="B1:C34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AMJ1048576" activeCellId="0" sqref="AMJ1048576"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.578125" defaultRowHeight="12.8" zeroHeight="true" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="1.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="59.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="1.26"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="0" width="30.86"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1024" min="6" style="0" width="11.56"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="1024" min="6" style="0" width="11.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -635,30 +638,30 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="n">
+        <v>800</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="9" t="n">
-        <v>101</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="9" t="n">
-        <v>200</v>
+        <v>101</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>24</v>
@@ -666,7 +669,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="9" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>25</v>
@@ -674,7 +677,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="9" t="n">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>26</v>
@@ -682,41 +685,49 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="9" t="n">
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="9" t="n">
+        <v>700</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14" t="n">
+      <c r="B31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="14" t="n">
         <v>100</v>
       </c>
-      <c r="C31" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="9" t="n">
+      <c r="C32" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="9" t="n">
         <v>200</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="C33" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:C2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>